<commit_message>
Actualización de documentación OF0348-Sp1
</commit_message>
<xml_diff>
--- a/OP0348-HU.xlsx
+++ b/OP0348-HU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\hubiC\PT\2018 PT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Documents\GitHub\OF0348-Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{232C735C-C862-4CA1-8A05-A337BE62305B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62361703-6BF4-4B37-BBAF-AD982B16F22E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de Usuario" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Ejemplo!$A$1:$K$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$K$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Historias de Usuario'!$A$1:$K$36</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="116">
   <si>
     <t>Rol</t>
   </si>
@@ -111,12 +111,6 @@
     <t>para autorizar el registro automatizado de identidades.</t>
   </si>
   <si>
-    <t>para llevar un control del uso de que se la a la red XMP</t>
-  </si>
-  <si>
-    <t>necesito visualizar por cada «credencial de consumidor» cuantas y que identidades han sido creadas por esta credencial</t>
-  </si>
-  <si>
     <t>OF0348-HU-01</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>debo poder registrarme automáticamente en «Openfire» usando credenciales de consumidor</t>
   </si>
   <si>
-    <t>para ser mejorar la seguridad de la comunicación y el servidor</t>
-  </si>
-  <si>
     <t>OF0348-HU-05</t>
   </si>
   <si>
@@ -183,33 +174,12 @@
     <t>cuando modifica una credencial</t>
   </si>
   <si>
-    <t>el sistema mostrará el cuadro de información "Modificación de credencial de Consumidor: Exitosa"</t>
-  </si>
-  <si>
-    <t>Visualización de credenciales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En caso que no existan consumer key </t>
-  </si>
-  <si>
-    <t>cuando se ingresa al modulo de configuración de registro</t>
-  </si>
-  <si>
-    <t>el sistema no mostrará ni una credencial de consumidor</t>
-  </si>
-  <si>
     <t>Sin identidades creadas</t>
   </si>
   <si>
     <t>Con identidades creadas</t>
   </si>
   <si>
-    <t>cuando se este la ventana de visualización de identidades</t>
-  </si>
-  <si>
-    <t>el sistema no mostrará una lista de identidades en la lista desplegable de texto</t>
-  </si>
-  <si>
     <t>Habilitar «Signing Forms»</t>
   </si>
   <si>
@@ -252,48 +222,27 @@
     <t>OF0348-HU: Historias de Usuario</t>
   </si>
   <si>
-    <t>el sistema mostrará el cuadro de información "Creación de credencial de Consumidor: Exitosa"</t>
-  </si>
-  <si>
-    <t>el sistema mostrará un cuadro de error: "Error: Credencial de Consumidor duplicada"</t>
-  </si>
-  <si>
     <t>Agregar credencial con valores inválidos</t>
   </si>
   <si>
     <t>En caso que se agreguen valores inválidos. Ej.: «n° de creación de identidades permitidas» = «fg&amp;»</t>
   </si>
   <si>
-    <t>el sistema mostrará un cuadro de  error: "Alguno de los valores ingresados es invalido"</t>
-  </si>
-  <si>
-    <t>para cambiar la cantidad de identidades asociadas a una credencial</t>
-  </si>
-  <si>
     <t>En caso que una credencial de consumidor no haya creado identidades</t>
   </si>
   <si>
     <t>En caso que una credencial de consumidor haya creado identidades</t>
   </si>
   <si>
-    <t>el sistema mostrará una lista  desplegable de texto en donde estarán las identidades creadas</t>
-  </si>
-  <si>
     <t>modificar valores de credencial con valores inválidos</t>
   </si>
   <si>
-    <t>En caso que se modifiquen valores inválidos. Ej.: «n° de creacción de identidades permitidas» = «fg&amp;»</t>
-  </si>
-  <si>
     <t>En caso que se habilite mediante un «radio button» la característica «Signing Forms» y se encuentre habilitada la característica «Registración In-Band»</t>
   </si>
   <si>
     <t>cuando guarde los cambios en la ventana de configuración de registro</t>
   </si>
   <si>
-    <t>el sistema permitirá registrar «Things» o clientes XMPP mediante el uso de «credenciales de consumidor»</t>
-  </si>
-  <si>
     <t>En caso que se deshabilite mediante un «radio button» la característica «Signing Forms» y se encuentre habilitada la característica «Registración In-Band»</t>
   </si>
   <si>
@@ -310,12 +259,126 @@
   </si>
   <si>
     <t>En caso que en el servidor este habilitado el registro «signing Forms» y la «Thing» lo esté utilizando estableciendo credenciales de consumidor invalidas.</t>
+  </si>
+  <si>
+    <t>En caso que se modifiquen valores inválidos. Ej.: «n° de creación de identidades permitidas» = «fg&amp;»</t>
+  </si>
+  <si>
+    <t>necesito visualizar  las «credenciales de consumidor», las identidades permitidas y las identidades utilizadas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para identificar el uso que cada consumidor hace de la red XMPP. </t>
+  </si>
+  <si>
+    <t>cuando el navegador se encuentre en la ventana de visualización de identidades</t>
+  </si>
+  <si>
+    <t>el sistema no mostrará una lista de identidades en la lista desplegable de texto.</t>
+  </si>
+  <si>
+    <t>OF0348-HU-07</t>
+  </si>
+  <si>
+    <t>OF0348-HU-08</t>
+  </si>
+  <si>
+    <t>necesito poder eliminar una identidad creada por una «credencial de consumidor»</t>
+  </si>
+  <si>
+    <t>Eliminar identidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En el caso que presione el boton eliminar de una identidad  </t>
+  </si>
+  <si>
+    <t>cuando me encuentre en la ventana de visualización de identidades asociada a una «credencial de consumidor»</t>
+  </si>
+  <si>
+    <t>el sistema deberá mostrar un cuadro de confirmación, para comprobar la eliminación de la identidad.</t>
+  </si>
+  <si>
+    <t>Cancelar borrado de identidad</t>
+  </si>
+  <si>
+    <t>En el caso que presione el boton eliminar de una identidad y luego cancele la eliminación</t>
+  </si>
+  <si>
+    <t>Aceptar borrado de identidad</t>
+  </si>
+  <si>
+    <t>En el caso que presione el boton eliminar de una identidad y luego acepte esta</t>
+  </si>
+  <si>
+    <t>El sistema deberá redirigirme a la pagina de visualización de identidades creadas por medio de «credenciales de consumidor», permaneciendo la identidad.</t>
+  </si>
+  <si>
+    <t>Sin identidades creadas con la «credencial de consumidor»</t>
+  </si>
+  <si>
+    <t>Con identidades creadas con la «credencial de consumidor»</t>
+  </si>
+  <si>
+    <t>para llevar un registro de las identidades creadas asociadas a una credencial de consumidor».</t>
+  </si>
+  <si>
+    <t>para tener la capacidad de eliminar un cliente malicioso que esta utilizando cierta identidad.</t>
+  </si>
+  <si>
+    <t>para cambiar la cantidad de identidades asociadas a una credencial.</t>
+  </si>
+  <si>
+    <t>para ser mejorar la seguridad de la comunicación y el servidor.</t>
+  </si>
+  <si>
+    <t>el sistema permitirá registrar «Things» o clientes XMPP mediante el uso de «credenciales de consumidor».</t>
+  </si>
+  <si>
+    <t>el sistema mostrará un cuadro de error: "Alguno de los valores ingresados es invalido".</t>
+  </si>
+  <si>
+    <t>el sistema mostrará el cuadro de información "Modificación de credencial de Consumidor: Exitosa".</t>
+  </si>
+  <si>
+    <t>el sistema mostrará un cuadro de  error: "Alguno de los valores ingresados es invalido".</t>
+  </si>
+  <si>
+    <t>el sistema mostrará un cuadro de error: «Error: Credencial de Consumidor duplicada».</t>
+  </si>
+  <si>
+    <t>el sistema mostrará el cuadro de información «Creación de credencial de Consumidor: Exitosa».</t>
+  </si>
+  <si>
+    <t>el sistema mostrará una lista desplegable de texto en donde estarán las identidades creadas.</t>
+  </si>
+  <si>
+    <t>cuando esté en la ventana de visualización de identidades</t>
+  </si>
+  <si>
+    <t>cuando acceda al visualizar las identidades creadas por medio de una «credencial de consumidor»</t>
+  </si>
+  <si>
+    <t>En el caso que no se hayan creado identidades</t>
+  </si>
+  <si>
+    <t>En el caso que se hayan creado identidades</t>
+  </si>
+  <si>
+    <t>El sistema no mostrará identidades.</t>
+  </si>
+  <si>
+    <t>El sistema mostrará las identidades creadas con anterioridad con la «credencial de consumidor» seleccionada.</t>
+  </si>
+  <si>
+    <t>El sistema deberá redirigirme a la pagina de visualización de identidades creadas por medio de «credenciales de consumidor», no listándose la identidad que borré.</t>
+  </si>
+  <si>
+    <t>necesito visualizar cuantas y que identidades han sido creadas con una «credencial de consumidor»</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,73 +571,73 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,597 +976,691 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="0.90625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="12.81640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" style="11" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="32.6328125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="25.08984375" style="11" customWidth="1"/>
-    <col min="10" max="10" width="39.08984375" style="11" customWidth="1"/>
-    <col min="11" max="11" width="3.1796875" style="11" customWidth="1"/>
-    <col min="12" max="16384" width="11.453125" style="11"/>
+    <col min="1" max="1" width="0.90625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.7265625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.1796875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="31.7265625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="25.08984375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="39.08984375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="3.1796875" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="11.453125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="18" x14ac:dyDescent="0.4">
-      <c r="B1" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
+      <c r="B1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F2" s="11"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="2:10" ht="18.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12" t="s">
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-    </row>
-    <row r="4" spans="2:10" ht="41.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+    </row>
+    <row r="4" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="13" t="s">
+      <c r="J4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="25" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="2:10" s="29" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" s="29" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="9">
+        <v>2</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" s="29" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="9">
+        <v>3</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+    </row>
+    <row r="9" spans="2:10" s="30" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" s="30" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="9">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+    </row>
+    <row r="12" spans="2:10" s="30" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="15">
+      <c r="C12" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="I5" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="J5" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15">
+      <c r="G12" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" s="30" customFormat="1" ht="65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="9">
         <v>2</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="25" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15">
-        <v>3</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="47.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15">
-        <v>4</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-    </row>
-    <row r="10" spans="2:10" ht="42.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="21" t="s">
+      <c r="G13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+    </row>
+    <row r="15" spans="2:10" s="30" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="15">
+      <c r="C15" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="F15" s="9">
         <v>1</v>
       </c>
-      <c r="G10" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B11" s="24"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="15">
+      <c r="G15" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" s="30" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="9">
         <v>2</v>
       </c>
-      <c r="G11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-    </row>
-    <row r="13" spans="2:10" ht="42.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="15">
+      <c r="G16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+    </row>
+    <row r="18" spans="2:10" s="30" customFormat="1" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H13" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="I13" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="15">
-        <v>2</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="I14" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="15">
-        <v>3</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="24"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="15">
-        <v>4</v>
-      </c>
-      <c r="G16" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="I16" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-    </row>
-    <row r="18" spans="2:10" ht="59.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F18" s="15">
-        <v>1</v>
-      </c>
-      <c r="G18" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="16" t="s">
+      <c r="G18" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="I18" s="16" t="s">
+      <c r="H18" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="I18" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="2:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="J18" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" s="30" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="15">
+      <c r="F19" s="9">
         <v>2</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="G19" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" s="30" customFormat="1" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="15">
+      <c r="F20" s="9">
         <v>3</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="16" t="s">
+      <c r="G20" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="I20" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J20" s="16" t="s">
+      <c r="H20" s="10" t="s">
         <v>91</v>
       </c>
+      <c r="I20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-    </row>
-    <row r="22" spans="2:10" ht="71" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+    </row>
+    <row r="22" spans="2:10" s="30" customFormat="1" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F22" s="15">
+      <c r="F22" s="9">
         <v>1</v>
       </c>
-      <c r="G22" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I22" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22" s="16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
+      <c r="G22" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" s="30" customFormat="1" ht="62.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="22"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
-      <c r="F23" s="15">
+      <c r="F23" s="9">
         <v>2</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="25"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
-    </row>
-    <row r="25" spans="2:10" ht="53" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="G23" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="H23" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="I23" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" s="30" customFormat="1" ht="37.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="22"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="9">
+        <v>3</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+    </row>
+    <row r="26" spans="2:10" ht="71" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+      <c r="F27" s="9">
+        <v>2</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B28" s="16"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="18"/>
+    </row>
+    <row r="29" spans="2:10" s="28" customFormat="1" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="F25" s="15">
+      <c r="D29" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="9">
         <v>1</v>
       </c>
-      <c r="G25" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="15">
+      <c r="G29" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I29" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" s="28" customFormat="1" ht="63.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="9">
         <v>2</v>
       </c>
-      <c r="G26" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="I26" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J26" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="27"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B30" s="29"/>
+      <c r="G30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I30" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B31" s="29"/>
+      <c r="B31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="18"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="12"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="D13:D16"/>
-    <mergeCell ref="E13:E16"/>
-    <mergeCell ref="B24:J24"/>
-    <mergeCell ref="B27:J27"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="B9:J9"/>
+  <mergeCells count="43">
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
     <mergeCell ref="B17:J17"/>
-    <mergeCell ref="B21:J21"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
-    <mergeCell ref="B5:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="B21:J21"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D26:D27"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="70" orientation="landscape" r:id="rId1"/>
@@ -1511,7 +1668,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J9"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
@@ -1545,18 +1702,18 @@
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
     </row>
     <row r="5" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
@@ -1588,16 +1745,16 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="58" x14ac:dyDescent="0.35">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="25" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="6">
@@ -1617,10 +1774,10 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
       <c r="F7" s="6">
         <v>2</v>
       </c>
@@ -1638,10 +1795,10 @@
       </c>
     </row>
     <row r="8" spans="2:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
       <c r="F8" s="6">
         <v>3</v>
       </c>
@@ -1659,10 +1816,10 @@
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
       <c r="F9" s="6"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>

</xml_diff>